<commit_message>
Prepare for testing dc converter
</commit_message>
<xml_diff>
--- a/Examples/IEEE_14Bus/IEEE_14Bus.xlsx
+++ b/Examples/IEEE_14Bus/IEEE_14Bus.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\IEEE_14Bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0CB63F-FF49-4C49-81F8-CC4A7AAF187A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14868B3-7624-4755-82C9-E305C0DB433A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PowerFlow" sheetId="1" r:id="rId1"/>
+    <sheet name="Bus" sheetId="1" r:id="rId1"/>
     <sheet name="Device" sheetId="3" r:id="rId2"/>
-    <sheet name="Basic" sheetId="4" r:id="rId3"/>
+    <sheet name="NetworkLine_IEEE" sheetId="5" r:id="rId3"/>
     <sheet name="NetworkLine" sheetId="2" r:id="rId4"/>
-    <sheet name="NetworkLine_IEEE Form" sheetId="5" r:id="rId5"/>
-    <sheet name="Advanced Setting" sheetId="6" r:id="rId6"/>
+    <sheet name="Basic" sheetId="4" r:id="rId5"/>
+    <sheet name="Advance" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>R (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -229,6 +229,14 @@
   </si>
   <si>
     <t>Turns Ratio (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area No.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC or DC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -604,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -617,12 +625,12 @@
     <col min="10" max="10" width="11.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -653,8 +661,14 @@
       <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -685,8 +699,14 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -723,8 +743,14 @@
         <f>50/100</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -759,8 +785,14 @@
         <f>40/100</f>
         <v>0.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -793,8 +825,14 @@
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -827,8 +865,14 @@
       <c r="J7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -864,8 +908,14 @@
         <f>24/100</f>
         <v>0.24</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -896,8 +946,14 @@
       <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -931,8 +987,14 @@
         <f>24/100</f>
         <v>0.24</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -965,8 +1027,14 @@
       <c r="J11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>10</v>
       </c>
@@ -999,8 +1067,14 @@
       <c r="J12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1033,8 +1107,14 @@
       <c r="J13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1067,8 +1147,14 @@
       <c r="J14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1101,8 +1187,14 @@
       <c r="J15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1134,6 +1226,12 @@
       </c>
       <c r="J16">
         <v>0</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1147,7 +1245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1364,56 +1462,525 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB93A31-1E5A-4104-8C10-8E6599437516}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D00B5E-E2E7-41B8-8388-8931D474EA96}">
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="18.53125" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15.796875" customWidth="1"/>
+    <col min="5" max="5" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1.9380000000000001E-2</v>
+      </c>
+      <c r="D6">
+        <v>5.917E-2</v>
+      </c>
+      <c r="E6">
+        <f>0.0528</f>
+        <v>5.28E-2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5.4030000000000002E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.22303999999999999</v>
+      </c>
+      <c r="E7">
+        <f>0.0492</f>
+        <v>4.9200000000000001E-2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>4.6989999999999997E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.19797000000000001</v>
+      </c>
+      <c r="E8">
+        <f>0.0438</f>
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>5.8110000000000002E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.17632</v>
+      </c>
+      <c r="E9">
+        <f>0.034</f>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>5.6950000000000001E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.17388000000000001</v>
+      </c>
+      <c r="E10">
+        <f>0.0346</f>
+        <v>3.4599999999999999E-2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>6.701E-2</v>
+      </c>
+      <c r="D11">
+        <v>0.17102999999999999</v>
+      </c>
+      <c r="E11">
+        <f>0.0128</f>
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>1.3350000000000001E-2</v>
+      </c>
+      <c r="D12">
+        <v>4.2110000000000002E-2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.20912</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0.97799999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.55618000000000001</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0.96899999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0.25202000000000002</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+      <c r="C16">
+        <v>9.4979999999999995E-2</v>
+      </c>
+      <c r="D16">
+        <v>0.19889999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
-        <f>B3*1000/2</f>
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5">
+      <c r="B17">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>0.12291000000000001</v>
+      </c>
+      <c r="D17">
+        <v>0.25580999999999998</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>6.615E-2</v>
+      </c>
+      <c r="D18">
+        <v>0.13027</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0.17615</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0.11001</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>3.1809999999999998E-2</v>
+      </c>
+      <c r="D21">
+        <v>8.4500000000000006E-2</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>14</v>
+      </c>
+      <c r="C22">
+        <v>0.12711</v>
+      </c>
+      <c r="D22">
+        <v>0.27038000000000001</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>8.2049999999999998E-2</v>
+      </c>
+      <c r="D23">
+        <v>0.19206999999999999</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>0.22092000000000001</v>
+      </c>
+      <c r="D24">
+        <v>0.19988</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>0.17093</v>
+      </c>
+      <c r="D25">
+        <v>0.34802</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
         <v>1</v>
       </c>
     </row>
@@ -1474,525 +2041,56 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D00B5E-E2E7-41B8-8388-8931D474EA96}">
-  <dimension ref="A1:G25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB93A31-1E5A-4104-8C10-8E6599437516}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.53125" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="18.53125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>1.9380000000000001E-2</v>
-      </c>
-      <c r="D6">
-        <v>5.917E-2</v>
-      </c>
-      <c r="E6">
-        <f>0.0528</f>
-        <v>5.28E-2</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>5.4030000000000002E-2</v>
-      </c>
-      <c r="D7">
-        <v>0.22303999999999999</v>
-      </c>
-      <c r="E7">
-        <f>0.0492</f>
-        <v>4.9200000000000001E-2</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>4.6989999999999997E-2</v>
-      </c>
-      <c r="D8">
-        <v>0.19797000000000001</v>
-      </c>
-      <c r="E8">
-        <f>0.0438</f>
-        <v>4.3799999999999999E-2</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>5.8110000000000002E-2</v>
-      </c>
-      <c r="D9">
-        <v>0.17632</v>
-      </c>
-      <c r="E9">
-        <f>0.034</f>
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>5.6950000000000001E-2</v>
-      </c>
-      <c r="D10">
-        <v>0.17388000000000001</v>
-      </c>
-      <c r="E10">
-        <f>0.0346</f>
-        <v>3.4599999999999999E-2</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>6.701E-2</v>
-      </c>
-      <c r="D11">
-        <v>0.17102999999999999</v>
-      </c>
-      <c r="E11">
-        <f>0.0128</f>
-        <v>1.2800000000000001E-2</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>1.3350000000000001E-2</v>
-      </c>
-      <c r="D12">
-        <v>4.2110000000000002E-2</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>7</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0.20912</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0.97799999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>9</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0.55618000000000001</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0.96899999999999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0.25202000000000002</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0.93200000000000005</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <v>11</v>
-      </c>
-      <c r="C16">
-        <v>9.4979999999999995E-2</v>
-      </c>
-      <c r="D16">
-        <v>0.19889999999999999</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17">
-        <v>12</v>
-      </c>
-      <c r="C17">
-        <v>0.12291000000000001</v>
-      </c>
-      <c r="D17">
-        <v>0.25580999999999998</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18">
-        <v>6</v>
-      </c>
-      <c r="B18">
-        <v>13</v>
-      </c>
-      <c r="C18">
-        <v>6.615E-2</v>
-      </c>
-      <c r="D18">
-        <v>0.13027</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A19">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <v>8</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0.17615</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A20">
-        <v>7</v>
-      </c>
-      <c r="B20">
-        <v>9</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0.11001</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A21">
-        <v>9</v>
-      </c>
-      <c r="B21">
-        <v>10</v>
-      </c>
-      <c r="C21">
-        <v>3.1809999999999998E-2</v>
-      </c>
-      <c r="D21">
-        <v>8.4500000000000006E-2</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A22">
-        <v>9</v>
-      </c>
-      <c r="B22">
-        <v>14</v>
-      </c>
-      <c r="C22">
-        <v>0.12711</v>
-      </c>
-      <c r="D22">
-        <v>0.27038000000000001</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23">
-        <v>10</v>
-      </c>
-      <c r="B23">
-        <v>11</v>
-      </c>
-      <c r="C23">
-        <v>8.2049999999999998E-2</v>
-      </c>
-      <c r="D23">
-        <v>0.19206999999999999</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A24">
-        <v>12</v>
-      </c>
-      <c r="B24">
-        <v>13</v>
-      </c>
-      <c r="C24">
-        <v>0.22092000000000001</v>
-      </c>
-      <c r="D24">
-        <v>0.19988</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25">
-        <v>13</v>
-      </c>
-      <c r="B25">
-        <v>14</v>
-      </c>
-      <c r="C25">
-        <v>0.17093</v>
-      </c>
-      <c r="D25">
-        <v>0.34802</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
+      <c r="B2" s="1">
+        <f>B3*1000/2</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
     </row>
@@ -2008,7 +2106,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2115,7 +2213,7 @@
         <v>45</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prepare for testing dc systems
The toolbox structure is changed and a lot of things are added, for testing dc networks: such as the netlist rearrangement, printing settings, port settings, etc.

A printing error for the strings of state, input, output of infinite bus is solved.
</commit_message>
<xml_diff>
--- a/Examples/IEEE_14Bus/IEEE_14Bus.xlsx
+++ b/Examples/IEEE_14Bus/IEEE_14Bus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\IEEE_14Bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14868B3-7624-4755-82C9-E305C0DB433A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F890AA8C-A115-4ECA-AE5A-56112F202654}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -614,7 +614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1245,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>

</xml_diff>